<commit_message>
Minor changes to clustering
</commit_message>
<xml_diff>
--- a/scrapped/Final data for clustering.xlsx
+++ b/scrapped/Final data for clustering.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>Specific rate of economic participation</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t># cities</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -494,6 +499,9 @@
       <c r="G2" t="n">
         <v>63.304197</v>
       </c>
+      <c r="H2" t="n">
+        <v>2022</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -519,6 +527,9 @@
       <c r="G3" t="n">
         <v>65.50967199999999</v>
       </c>
+      <c r="H3" t="n">
+        <v>5545</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -544,6 +555,9 @@
       <c r="G4" t="n">
         <v>67.045768</v>
       </c>
+      <c r="H4" t="n">
+        <v>2543</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -569,6 +583,9 @@
       <c r="G5" t="n">
         <v>63.341754</v>
       </c>
+      <c r="H5" t="n">
+        <v>2762</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -594,6 +611,9 @@
       <c r="G6" t="n">
         <v>61.18854</v>
       </c>
+      <c r="H6" t="n">
+        <v>21157</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -619,6 +639,9 @@
       <c r="G7" t="n">
         <v>62.272983</v>
       </c>
+      <c r="H7" t="n">
+        <v>12186</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -644,6 +667,9 @@
       <c r="G8" t="n">
         <v>59.986685</v>
       </c>
+      <c r="H8" t="n">
+        <v>4034</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -669,6 +695,9 @@
       <c r="G9" t="n">
         <v>65.26616799999999</v>
       </c>
+      <c r="H9" t="n">
+        <v>1226</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -694,6 +723,9 @@
       <c r="G10" t="n">
         <v>64.430013</v>
       </c>
+      <c r="H10" t="n">
+        <v>634</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -719,6 +751,9 @@
       <c r="G11" t="n">
         <v>57.783127</v>
       </c>
+      <c r="H11" t="n">
+        <v>5890</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -744,6 +779,9 @@
       <c r="G12" t="n">
         <v>61.838603</v>
       </c>
+      <c r="H12" t="n">
+        <v>8809</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -769,6 +807,9 @@
       <c r="G13" t="n">
         <v>60.590712</v>
       </c>
+      <c r="H13" t="n">
+        <v>6769</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -794,6 +835,9 @@
       <c r="G14" t="n">
         <v>61.111455</v>
       </c>
+      <c r="H14" t="n">
+        <v>4690</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -819,6 +863,9 @@
       <c r="G15" t="n">
         <v>64.102896</v>
       </c>
+      <c r="H15" t="n">
+        <v>10348</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -844,6 +891,9 @@
       <c r="G16" t="n">
         <v>62.173551</v>
       </c>
+      <c r="H16" t="n">
+        <v>4894</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -869,6 +919,9 @@
       <c r="G17" t="n">
         <v>62.061083</v>
       </c>
+      <c r="H17" t="n">
+        <v>8644</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -894,6 +947,9 @@
       <c r="G18" t="n">
         <v>63.59053</v>
       </c>
+      <c r="H18" t="n">
+        <v>1578</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -919,6 +975,9 @@
       <c r="G19" t="n">
         <v>62.795767</v>
       </c>
+      <c r="H19" t="n">
+        <v>2850</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -944,6 +1003,9 @@
       <c r="G20" t="n">
         <v>61.421171</v>
       </c>
+      <c r="H20" t="n">
+        <v>4822</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -969,6 +1031,9 @@
       <c r="G21" t="n">
         <v>56.780517</v>
       </c>
+      <c r="H21" t="n">
+        <v>10723</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -994,6 +1059,9 @@
       <c r="G22" t="n">
         <v>61.98869</v>
       </c>
+      <c r="H22" t="n">
+        <v>6568</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1019,6 +1087,9 @@
       <c r="G23" t="n">
         <v>65.031097</v>
       </c>
+      <c r="H23" t="n">
+        <v>2192</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1044,6 +1115,9 @@
       <c r="G24" t="n">
         <v>68.471808</v>
       </c>
+      <c r="H24" t="n">
+        <v>2207</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1069,6 +1143,9 @@
       <c r="G25" t="n">
         <v>60.623926</v>
       </c>
+      <c r="H25" t="n">
+        <v>6554</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1094,6 +1171,9 @@
       <c r="G26" t="n">
         <v>60.621923</v>
       </c>
+      <c r="H26" t="n">
+        <v>5495</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1119,6 +1199,9 @@
       <c r="G27" t="n">
         <v>60.999538</v>
       </c>
+      <c r="H27" t="n">
+        <v>7300</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1144,6 +1227,9 @@
       <c r="G28" t="n">
         <v>62.337791</v>
       </c>
+      <c r="H28" t="n">
+        <v>2472</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1169,6 +1255,9 @@
       <c r="G29" t="n">
         <v>61.334601</v>
       </c>
+      <c r="H29" t="n">
+        <v>6566</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1194,6 +1283,9 @@
       <c r="G30" t="n">
         <v>61.018407</v>
       </c>
+      <c r="H30" t="n">
+        <v>1175</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1219,6 +1311,9 @@
       <c r="G31" t="n">
         <v>59.162221</v>
       </c>
+      <c r="H31" t="n">
+        <v>19845</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1244,6 +1339,9 @@
       <c r="G32" t="n">
         <v>61.740748</v>
       </c>
+      <c r="H32" t="n">
+        <v>2434</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1268,6 +1366,9 @@
       </c>
       <c r="G33" t="n">
         <v>56.027752</v>
+      </c>
+      <c r="H33" t="n">
+        <v>4498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>